<commit_message>
all daily box office $ scraped
</commit_message>
<xml_diff>
--- a/1-american-sniper/american-sniper.xlsx
+++ b/1-american-sniper/american-sniper.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/paperback-nonfiction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/1-american-sniper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9B766061-FD98-B447-B545-43A35519A071}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14F3EAA5-B812-DA4F-90E8-828E6D383FEE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="3320" windowWidth="18600" windowHeight="21920" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
+    <workbookView xWindow="26320" yWindow="2060" windowWidth="22380" windowHeight="21920" activeTab="1" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NYT Books" sheetId="1" r:id="rId1"/>
+    <sheet name="Box Office" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="9">
   <si>
     <t>Published Date</t>
   </si>
@@ -47,13 +48,20 @@
   <si>
     <t>Movie Opens: 2015-12-25</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Gross</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,13 +104,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE81FAE-AFF2-424B-B98F-EB8EE3D8F204}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A81" workbookViewId="0">
       <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
@@ -2463,4 +2472,1496 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5013F2-7369-4142-97F8-212C34FA103F}">
+  <dimension ref="A1:B184"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>41998</v>
+      </c>
+      <c r="B2" s="6">
+        <v>240211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>41999</v>
+      </c>
+      <c r="B3" s="6">
+        <v>199481</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>42000</v>
+      </c>
+      <c r="B4" s="6">
+        <v>215858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42001</v>
+      </c>
+      <c r="B5" s="6">
+        <v>218117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42002</v>
+      </c>
+      <c r="B6" s="6">
+        <v>166444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>42003</v>
+      </c>
+      <c r="B7" s="6">
+        <v>164201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>42004</v>
+      </c>
+      <c r="B8" s="6">
+        <v>124987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B9" s="6">
+        <v>223080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>42006</v>
+      </c>
+      <c r="B10" s="6">
+        <v>233719</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42007</v>
+      </c>
+      <c r="B11" s="6">
+        <v>238862</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42008</v>
+      </c>
+      <c r="B12" s="6">
+        <v>204328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>42009</v>
+      </c>
+      <c r="B13" s="6">
+        <v>100505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>42010</v>
+      </c>
+      <c r="B14" s="6">
+        <v>89058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>42011</v>
+      </c>
+      <c r="B15" s="6">
+        <v>93332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>42012</v>
+      </c>
+      <c r="B16" s="6">
+        <v>82968</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>42013</v>
+      </c>
+      <c r="B17" s="6">
+        <v>156360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>42014</v>
+      </c>
+      <c r="B18" s="6">
+        <v>234210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>42015</v>
+      </c>
+      <c r="B19" s="6">
+        <v>188948</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>42016</v>
+      </c>
+      <c r="B20" s="6">
+        <v>60183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>42017</v>
+      </c>
+      <c r="B21" s="6">
+        <v>68600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>42018</v>
+      </c>
+      <c r="B22" s="6">
+        <v>69270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>42019</v>
+      </c>
+      <c r="B23" s="6">
+        <v>52056</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>42020</v>
+      </c>
+      <c r="B24" s="6">
+        <v>30338488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>42021</v>
+      </c>
+      <c r="B25" s="6">
+        <v>34547284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>42022</v>
+      </c>
+      <c r="B26" s="6">
+        <v>24383294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>42023</v>
+      </c>
+      <c r="B27" s="6">
+        <v>17942391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>42024</v>
+      </c>
+      <c r="B28" s="6">
+        <v>9924117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>42025</v>
+      </c>
+      <c r="B29" s="6">
+        <v>7555269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>42026</v>
+      </c>
+      <c r="B30" s="6">
+        <v>7656492</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>42027</v>
+      </c>
+      <c r="B31" s="6">
+        <v>18213554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>42028</v>
+      </c>
+      <c r="B32" s="6">
+        <v>28635135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>42029</v>
+      </c>
+      <c r="B33" s="6">
+        <v>17779615</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>42030</v>
+      </c>
+      <c r="B34" s="6">
+        <v>4183367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>42031</v>
+      </c>
+      <c r="B35" s="6">
+        <v>5017038</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>42032</v>
+      </c>
+      <c r="B36" s="6">
+        <v>3823135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>42033</v>
+      </c>
+      <c r="B37" s="6">
+        <v>3668056</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>42034</v>
+      </c>
+      <c r="B38" s="6">
+        <v>9905616</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>42035</v>
+      </c>
+      <c r="B39" s="6">
+        <v>16510536</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B40" s="6">
+        <v>4244376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>42037</v>
+      </c>
+      <c r="B41" s="6">
+        <v>2645109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>42038</v>
+      </c>
+      <c r="B42" s="6">
+        <v>2923141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42039</v>
+      </c>
+      <c r="B43" s="6">
+        <v>2273342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42040</v>
+      </c>
+      <c r="B44" s="6">
+        <v>2506106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>42041</v>
+      </c>
+      <c r="B45" s="6">
+        <v>6163365</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>42042</v>
+      </c>
+      <c r="B46" s="6">
+        <v>11032447</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>42043</v>
+      </c>
+      <c r="B47" s="6">
+        <v>6093301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>42044</v>
+      </c>
+      <c r="B48" s="6">
+        <v>1590242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>42045</v>
+      </c>
+      <c r="B49" s="6">
+        <v>1773361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>42046</v>
+      </c>
+      <c r="B50" s="6">
+        <v>1468160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>42047</v>
+      </c>
+      <c r="B51" s="6">
+        <v>1477178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>42048</v>
+      </c>
+      <c r="B52" s="6">
+        <v>3745563</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>42049</v>
+      </c>
+      <c r="B53" s="6">
+        <v>7824072</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>42050</v>
+      </c>
+      <c r="B54" s="6">
+        <v>4845170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>42051</v>
+      </c>
+      <c r="B55" s="6">
+        <v>2365038</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>42052</v>
+      </c>
+      <c r="B56" s="6">
+        <v>1284385</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>42053</v>
+      </c>
+      <c r="B57" s="6">
+        <v>1037497</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>42054</v>
+      </c>
+      <c r="B58" s="6">
+        <v>1157160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>42055</v>
+      </c>
+      <c r="B59" s="6">
+        <v>2718122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>42056</v>
+      </c>
+      <c r="B60" s="6">
+        <v>4595743</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>42057</v>
+      </c>
+      <c r="B61" s="6">
+        <v>2738582</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>42058</v>
+      </c>
+      <c r="B62" s="6">
+        <v>836221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>42059</v>
+      </c>
+      <c r="B63" s="6">
+        <v>948496</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>42060</v>
+      </c>
+      <c r="B64" s="6">
+        <v>792101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>42061</v>
+      </c>
+      <c r="B65" s="6">
+        <v>822004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>42062</v>
+      </c>
+      <c r="B66" s="6">
+        <v>1903469</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>42063</v>
+      </c>
+      <c r="B67" s="6">
+        <v>3601727</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B68" s="6">
+        <v>1889097</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>42065</v>
+      </c>
+      <c r="B69" s="6">
+        <v>502179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>42066</v>
+      </c>
+      <c r="B70" s="6">
+        <v>507318</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>42067</v>
+      </c>
+      <c r="B71" s="6">
+        <v>429402</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>42068</v>
+      </c>
+      <c r="B72" s="6">
+        <v>457340</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>42069</v>
+      </c>
+      <c r="B73" s="6">
+        <v>1146840</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>42070</v>
+      </c>
+      <c r="B74" s="6">
+        <v>2158539</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>42071</v>
+      </c>
+      <c r="B75" s="6">
+        <v>1096012</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>42072</v>
+      </c>
+      <c r="B76" s="6">
+        <v>342258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>42073</v>
+      </c>
+      <c r="B77" s="6">
+        <v>409581</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>42074</v>
+      </c>
+      <c r="B78" s="6">
+        <v>363324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>42075</v>
+      </c>
+      <c r="B79" s="6">
+        <v>354030</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>42076</v>
+      </c>
+      <c r="B80" s="6">
+        <v>755768</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>42077</v>
+      </c>
+      <c r="B81" s="6">
+        <v>1382406</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>42078</v>
+      </c>
+      <c r="B82" s="6">
+        <v>673168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>42079</v>
+      </c>
+      <c r="B83" s="6">
+        <v>232068</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>42080</v>
+      </c>
+      <c r="B84" s="6">
+        <v>255383</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>42081</v>
+      </c>
+      <c r="B85" s="6">
+        <v>256310</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>42082</v>
+      </c>
+      <c r="B86" s="6">
+        <v>236086</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>42083</v>
+      </c>
+      <c r="B87" s="6">
+        <v>432738</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>42084</v>
+      </c>
+      <c r="B88" s="6">
+        <v>785413</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>42085</v>
+      </c>
+      <c r="B89" s="6">
+        <v>390100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>42086</v>
+      </c>
+      <c r="B90" s="6">
+        <v>152393</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>42087</v>
+      </c>
+      <c r="B91" s="6">
+        <v>155245</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>42088</v>
+      </c>
+      <c r="B92" s="6">
+        <v>137446</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>42089</v>
+      </c>
+      <c r="B93" s="6">
+        <v>126147</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>42090</v>
+      </c>
+      <c r="B94" s="6">
+        <v>246937</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>42091</v>
+      </c>
+      <c r="B95" s="6">
+        <v>423874</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>42092</v>
+      </c>
+      <c r="B96" s="6">
+        <v>203242</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>42093</v>
+      </c>
+      <c r="B97" s="6">
+        <v>81213</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>42094</v>
+      </c>
+      <c r="B98" s="6">
+        <v>91324</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B99" s="6">
+        <v>83249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>42096</v>
+      </c>
+      <c r="B100" s="6">
+        <v>88355</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>42097</v>
+      </c>
+      <c r="B101" s="6">
+        <v>230878</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>42098</v>
+      </c>
+      <c r="B102" s="6">
+        <v>261490</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>42099</v>
+      </c>
+      <c r="B103" s="6">
+        <v>135692</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>42100</v>
+      </c>
+      <c r="B104" s="6">
+        <v>55473</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>42101</v>
+      </c>
+      <c r="B105" s="6">
+        <v>61575</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>42102</v>
+      </c>
+      <c r="B106" s="6">
+        <v>55517</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>42103</v>
+      </c>
+      <c r="B107" s="6">
+        <v>57183</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B108" s="6">
+        <v>180278</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>42105</v>
+      </c>
+      <c r="B109" s="6">
+        <v>302268</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>42106</v>
+      </c>
+      <c r="B110" s="6">
+        <v>112495</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>42107</v>
+      </c>
+      <c r="B111" s="6">
+        <v>40555</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>42108</v>
+      </c>
+      <c r="B112" s="6">
+        <v>48387</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>42109</v>
+      </c>
+      <c r="B113" s="6">
+        <v>44459</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>42110</v>
+      </c>
+      <c r="B114" s="6">
+        <v>38505</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>42111</v>
+      </c>
+      <c r="B115" s="6">
+        <v>104872</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>42112</v>
+      </c>
+      <c r="B116" s="6">
+        <v>185191</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>42113</v>
+      </c>
+      <c r="B117" s="6">
+        <v>89655</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>42114</v>
+      </c>
+      <c r="B118" s="6">
+        <v>37173</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>42115</v>
+      </c>
+      <c r="B119" s="6">
+        <v>42393</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>42116</v>
+      </c>
+      <c r="B120" s="6">
+        <v>37243</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>42117</v>
+      </c>
+      <c r="B121" s="6">
+        <v>40967</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>42118</v>
+      </c>
+      <c r="B122" s="6">
+        <v>96576</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>42119</v>
+      </c>
+      <c r="B123" s="6">
+        <v>187408</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>42120</v>
+      </c>
+      <c r="B124" s="6">
+        <v>90615</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>42121</v>
+      </c>
+      <c r="B125" s="6">
+        <v>31715</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>42122</v>
+      </c>
+      <c r="B126" s="6">
+        <v>34857</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>42123</v>
+      </c>
+      <c r="B127" s="6">
+        <v>29628</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>42124</v>
+      </c>
+      <c r="B128" s="6">
+        <v>26072</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B129" s="6">
+        <v>123899</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>42126</v>
+      </c>
+      <c r="B130" s="6">
+        <v>171757</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>42127</v>
+      </c>
+      <c r="B131" s="6">
+        <v>148259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>42128</v>
+      </c>
+      <c r="B132" s="6">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>42129</v>
+      </c>
+      <c r="B133" s="6">
+        <v>50556</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>42130</v>
+      </c>
+      <c r="B134" s="6">
+        <v>39939</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>42131</v>
+      </c>
+      <c r="B135" s="6">
+        <v>35947</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>42132</v>
+      </c>
+      <c r="B136" s="6">
+        <v>86330</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>42133</v>
+      </c>
+      <c r="B137" s="6">
+        <v>119155</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>42134</v>
+      </c>
+      <c r="B138" s="6">
+        <v>85256</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>42135</v>
+      </c>
+      <c r="B139" s="6">
+        <v>34102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>42136</v>
+      </c>
+      <c r="B140" s="6">
+        <v>37513</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>42137</v>
+      </c>
+      <c r="B141" s="6">
+        <v>28134</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>42138</v>
+      </c>
+      <c r="B142" s="6">
+        <v>27572</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>42139</v>
+      </c>
+      <c r="B143" s="6">
+        <v>54584</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>42140</v>
+      </c>
+      <c r="B144" s="6">
+        <v>88711</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>42141</v>
+      </c>
+      <c r="B145" s="6">
+        <v>45686</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>42142</v>
+      </c>
+      <c r="B146" s="6">
+        <v>15890</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>42143</v>
+      </c>
+      <c r="B147" s="6">
+        <v>17002</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>42144</v>
+      </c>
+      <c r="B148" s="6">
+        <v>16151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>42145</v>
+      </c>
+      <c r="B149" s="6">
+        <v>19120</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>42146</v>
+      </c>
+      <c r="B150" s="6">
+        <v>43350</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>42147</v>
+      </c>
+      <c r="B151" s="6">
+        <v>69227</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>42148</v>
+      </c>
+      <c r="B152" s="6">
+        <v>72440</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>42149</v>
+      </c>
+      <c r="B153" s="6">
+        <v>42529</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>42150</v>
+      </c>
+      <c r="B154" s="6">
+        <v>13184</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>42151</v>
+      </c>
+      <c r="B155" s="6">
+        <v>10942</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>42152</v>
+      </c>
+      <c r="B156" s="6">
+        <v>12364</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>42153</v>
+      </c>
+      <c r="B157" s="6">
+        <v>19029</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>42154</v>
+      </c>
+      <c r="B158" s="6">
+        <v>28047</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>42155</v>
+      </c>
+      <c r="B159" s="6">
+        <v>20327</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B160" s="6">
+        <v>6327</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>42157</v>
+      </c>
+      <c r="B161" s="6">
+        <v>7076</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>42158</v>
+      </c>
+      <c r="B162" s="6">
+        <v>6651</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>42159</v>
+      </c>
+      <c r="B163" s="6">
+        <v>6317</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>42160</v>
+      </c>
+      <c r="B164" s="6">
+        <v>6531</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>42161</v>
+      </c>
+      <c r="B165" s="6">
+        <v>10859</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>42162</v>
+      </c>
+      <c r="B166" s="6">
+        <v>5757</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>42163</v>
+      </c>
+      <c r="B167" s="6">
+        <v>2497</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>42164</v>
+      </c>
+      <c r="B168" s="6">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>42165</v>
+      </c>
+      <c r="B169" s="6">
+        <v>2651</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>42166</v>
+      </c>
+      <c r="B170" s="6">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>42167</v>
+      </c>
+      <c r="B171" s="6">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>42168</v>
+      </c>
+      <c r="B172" s="6">
+        <v>5228</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>42169</v>
+      </c>
+      <c r="B173" s="6">
+        <v>3292</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>42170</v>
+      </c>
+      <c r="B174" s="6">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>42171</v>
+      </c>
+      <c r="B175" s="6">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>42172</v>
+      </c>
+      <c r="B176" s="6">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>42173</v>
+      </c>
+      <c r="B177" s="6">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>42174</v>
+      </c>
+      <c r="B178" s="6">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>42175</v>
+      </c>
+      <c r="B179" s="6">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>42176</v>
+      </c>
+      <c r="B180" s="6">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>42177</v>
+      </c>
+      <c r="B181" s="6">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>42178</v>
+      </c>
+      <c r="B182" s="6">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>42179</v>
+      </c>
+      <c r="B183" s="6">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>42180</v>
+      </c>
+      <c r="B184" s="6">
+        <v>789</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
weekly box office data
</commit_message>
<xml_diff>
--- a/1-american-sniper/american-sniper.xlsx
+++ b/1-american-sniper/american-sniper.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/1-american-sniper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{14F3EAA5-B812-DA4F-90E8-828E6D383FEE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6C225C6D-CECD-FB43-8F87-8D94EAD46A0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26320" yWindow="2060" windowWidth="22380" windowHeight="21920" activeTab="1" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
+    <workbookView xWindow="2360" yWindow="4160" windowWidth="22380" windowHeight="21920" activeTab="2" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
   </bookViews>
   <sheets>
     <sheet name="NYT Books" sheetId="1" r:id="rId1"/>
     <sheet name="Box Office" sheetId="2" r:id="rId2"/>
+    <sheet name="Weekly Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="12">
   <si>
     <t>Published Date</t>
   </si>
@@ -53,6 +54,15 @@
   </si>
   <si>
     <t>Gross</t>
+  </si>
+  <si>
+    <t>Week Start</t>
+  </si>
+  <si>
+    <t>Week End</t>
+  </si>
+  <si>
+    <t>Box Office Gross</t>
   </si>
 </sst>
 </file>
@@ -428,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE81FAE-AFF2-424B-B98F-EB8EE3D8F204}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2478,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5013F2-7369-4142-97F8-212C34FA103F}">
   <dimension ref="A1:B184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3964,4 +3974,1752 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A462E3-9853-A64F-9EF3-EF62BAAD9838}">
+  <dimension ref="A1:D135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D128" sqref="D128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <f>B2-6</f>
+        <v>41301</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41307</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>B3-6</f>
+        <v>41308</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41314</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">B4-6</f>
+        <v>41315</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41321</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>41322</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41328</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>41329</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41335</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>41336</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41342</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>41343</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41349</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>41350</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41356</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>41357</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41363</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>41364</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41370</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>41371</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41377</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>41378</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41384</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>41385</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41391</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>41392</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41398</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>41399</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41405</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>41406</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41412</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>41413</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41419</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>41420</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41426</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>41427</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41433</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>41434</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41440</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>41441</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41447</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>41448</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41454</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>41455</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41461</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>41462</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41468</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>41469</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41475</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>41476</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41482</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>41483</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41489</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>41490</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41496</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>41497</v>
+      </c>
+      <c r="B30" s="1">
+        <v>41503</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>41504</v>
+      </c>
+      <c r="B31" s="1">
+        <v>41510</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>41511</v>
+      </c>
+      <c r="B32" s="1">
+        <v>41517</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>41518</v>
+      </c>
+      <c r="B33" s="1">
+        <v>41524</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>41525</v>
+      </c>
+      <c r="B34" s="1">
+        <v>41531</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>41532</v>
+      </c>
+      <c r="B35" s="1">
+        <v>41538</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>41539</v>
+      </c>
+      <c r="B36" s="1">
+        <v>41545</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>41546</v>
+      </c>
+      <c r="B37" s="1">
+        <v>41552</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>41553</v>
+      </c>
+      <c r="B38" s="1">
+        <v>41559</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>41560</v>
+      </c>
+      <c r="B39" s="1">
+        <v>41566</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>41567</v>
+      </c>
+      <c r="B40" s="1">
+        <v>41573</v>
+      </c>
+      <c r="C40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>41574</v>
+      </c>
+      <c r="B41" s="1">
+        <v>41580</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>41581</v>
+      </c>
+      <c r="B42" s="1">
+        <v>41587</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>41588</v>
+      </c>
+      <c r="B43" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>41595</v>
+      </c>
+      <c r="B44" s="1">
+        <v>41601</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>41602</v>
+      </c>
+      <c r="B45" s="1">
+        <v>41608</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>41609</v>
+      </c>
+      <c r="B46" s="1">
+        <v>41615</v>
+      </c>
+      <c r="C46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>41616</v>
+      </c>
+      <c r="B47" s="1">
+        <v>41622</v>
+      </c>
+      <c r="C47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>41623</v>
+      </c>
+      <c r="B48" s="1">
+        <v>41629</v>
+      </c>
+      <c r="C48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>41630</v>
+      </c>
+      <c r="B49" s="1">
+        <v>41636</v>
+      </c>
+      <c r="C49">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>41637</v>
+      </c>
+      <c r="B50" s="1">
+        <v>41643</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>41644</v>
+      </c>
+      <c r="B51" s="1">
+        <v>41650</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>41651</v>
+      </c>
+      <c r="B52" s="1">
+        <v>41657</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>41658</v>
+      </c>
+      <c r="B53" s="1">
+        <v>41664</v>
+      </c>
+      <c r="C53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>41665</v>
+      </c>
+      <c r="B54" s="1">
+        <v>41671</v>
+      </c>
+      <c r="C54">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>41672</v>
+      </c>
+      <c r="B55" s="1">
+        <v>41678</v>
+      </c>
+      <c r="C55">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>41679</v>
+      </c>
+      <c r="B56" s="1">
+        <v>41685</v>
+      </c>
+      <c r="C56">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>41686</v>
+      </c>
+      <c r="B57" s="1">
+        <v>41692</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="B58" s="1">
+        <v>41699</v>
+      </c>
+      <c r="C58">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>41700</v>
+      </c>
+      <c r="B59" s="1">
+        <v>41706</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>41707</v>
+      </c>
+      <c r="B60" s="1">
+        <v>41713</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="B61" s="1">
+        <v>41720</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="B62" s="1">
+        <v>41727</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>41728</v>
+      </c>
+      <c r="B63" s="1">
+        <v>41734</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>41735</v>
+      </c>
+      <c r="B64" s="1">
+        <v>41741</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>41742</v>
+      </c>
+      <c r="B65" s="1">
+        <v>41748</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>41749</v>
+      </c>
+      <c r="B66" s="1">
+        <v>41755</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>41756</v>
+      </c>
+      <c r="B67" s="1">
+        <v>41762</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A131" si="1">B68-6</f>
+        <v>41763</v>
+      </c>
+      <c r="B68" s="1">
+        <v>41769</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>41770</v>
+      </c>
+      <c r="B69" s="1">
+        <v>41776</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>41777</v>
+      </c>
+      <c r="B70" s="1">
+        <v>41783</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>41784</v>
+      </c>
+      <c r="B71" s="1">
+        <v>41790</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>41791</v>
+      </c>
+      <c r="B72" s="1">
+        <v>41797</v>
+      </c>
+      <c r="C72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>41798</v>
+      </c>
+      <c r="B73" s="1">
+        <v>41804</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>41805</v>
+      </c>
+      <c r="B74" s="1">
+        <v>41811</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>41812</v>
+      </c>
+      <c r="B75" s="1">
+        <v>41818</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>41819</v>
+      </c>
+      <c r="B76" s="1">
+        <v>41825</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>41826</v>
+      </c>
+      <c r="B77" s="1">
+        <v>41832</v>
+      </c>
+      <c r="C77" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>41833</v>
+      </c>
+      <c r="B78" s="1">
+        <v>41839</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>41840</v>
+      </c>
+      <c r="B79" s="1">
+        <v>41846</v>
+      </c>
+      <c r="C79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>41847</v>
+      </c>
+      <c r="B80" s="1">
+        <v>41853</v>
+      </c>
+      <c r="C80">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>41854</v>
+      </c>
+      <c r="B81" s="1">
+        <v>41860</v>
+      </c>
+      <c r="C81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>41861</v>
+      </c>
+      <c r="B82" s="1">
+        <v>41867</v>
+      </c>
+      <c r="C82" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>41868</v>
+      </c>
+      <c r="B83" s="1">
+        <v>41874</v>
+      </c>
+      <c r="C83">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>41875</v>
+      </c>
+      <c r="B84" s="1">
+        <v>41881</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>41882</v>
+      </c>
+      <c r="B85" s="1">
+        <v>41888</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>41889</v>
+      </c>
+      <c r="B86" s="1">
+        <v>41895</v>
+      </c>
+      <c r="C86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>41896</v>
+      </c>
+      <c r="B87" s="1">
+        <v>41902</v>
+      </c>
+      <c r="C87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>41903</v>
+      </c>
+      <c r="B88" s="1">
+        <v>41909</v>
+      </c>
+      <c r="C88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>41910</v>
+      </c>
+      <c r="B89" s="1">
+        <v>41916</v>
+      </c>
+      <c r="C89">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>41917</v>
+      </c>
+      <c r="B90" s="1">
+        <v>41923</v>
+      </c>
+      <c r="C90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>41924</v>
+      </c>
+      <c r="B91" s="1">
+        <v>41930</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>41931</v>
+      </c>
+      <c r="B92" s="1">
+        <v>41937</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <f t="shared" si="1"/>
+        <v>41938</v>
+      </c>
+      <c r="B93" s="1">
+        <v>41944</v>
+      </c>
+      <c r="C93">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <f t="shared" si="1"/>
+        <v>41945</v>
+      </c>
+      <c r="B94" s="1">
+        <v>41951</v>
+      </c>
+      <c r="C94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <f t="shared" si="1"/>
+        <v>41952</v>
+      </c>
+      <c r="B95" s="1">
+        <v>41958</v>
+      </c>
+      <c r="C95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <f t="shared" si="1"/>
+        <v>41959</v>
+      </c>
+      <c r="B96" s="1">
+        <v>41965</v>
+      </c>
+      <c r="C96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <f t="shared" si="1"/>
+        <v>41966</v>
+      </c>
+      <c r="B97" s="1">
+        <v>41972</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <f t="shared" si="1"/>
+        <v>41973</v>
+      </c>
+      <c r="B98" s="1">
+        <v>41979</v>
+      </c>
+      <c r="C98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <f t="shared" si="1"/>
+        <v>41980</v>
+      </c>
+      <c r="B99" s="1">
+        <v>41986</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <f t="shared" si="1"/>
+        <v>41987</v>
+      </c>
+      <c r="B100" s="1">
+        <v>41993</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <f t="shared" si="1"/>
+        <v>41994</v>
+      </c>
+      <c r="B101" s="1">
+        <v>42000</v>
+      </c>
+      <c r="C101">
+        <v>3</v>
+      </c>
+      <c r="D101" s="6">
+        <f>SUM('Box Office'!B2:B4)</f>
+        <v>655550</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <f t="shared" si="1"/>
+        <v>42001</v>
+      </c>
+      <c r="B102" s="1">
+        <v>42007</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" s="6">
+        <f>SUM('Box Office'!B5:B11)</f>
+        <v>1369410</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <f t="shared" si="1"/>
+        <v>42008</v>
+      </c>
+      <c r="B103" s="1">
+        <v>42014</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" s="6">
+        <f>SUM('Box Office'!B12:B18)</f>
+        <v>960761</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <f t="shared" si="1"/>
+        <v>42015</v>
+      </c>
+      <c r="B104" s="1">
+        <v>42021</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104" s="6">
+        <f>SUM('Box Office'!B19:B25)</f>
+        <v>65324829</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <f t="shared" si="1"/>
+        <v>42022</v>
+      </c>
+      <c r="B105" s="1">
+        <v>42028</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" s="6">
+        <f>SUM('Box Office'!B26:B32)</f>
+        <v>114310252</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <f t="shared" si="1"/>
+        <v>42029</v>
+      </c>
+      <c r="B106" s="1">
+        <v>42035</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106" s="6">
+        <f>SUM('Box Office'!B33:B39)</f>
+        <v>60887363</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <f t="shared" si="1"/>
+        <v>42036</v>
+      </c>
+      <c r="B107" s="1">
+        <v>42042</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107" s="6">
+        <f>SUM('Box Office'!B40:B46)</f>
+        <v>31787886</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <f t="shared" si="1"/>
+        <v>42043</v>
+      </c>
+      <c r="B108" s="1">
+        <v>42049</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" s="6">
+        <f>SUM('Box Office'!B47:B53)</f>
+        <v>23971877</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <f t="shared" si="1"/>
+        <v>42050</v>
+      </c>
+      <c r="B109" s="1">
+        <v>42056</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" s="6">
+        <f>SUM('Box Office'!B54:B60)</f>
+        <v>18003115</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <f t="shared" si="1"/>
+        <v>42057</v>
+      </c>
+      <c r="B110" s="1">
+        <v>42063</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" s="6">
+        <f>SUM('Box Office'!B61:B67)</f>
+        <v>11642600</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <f t="shared" si="1"/>
+        <v>42064</v>
+      </c>
+      <c r="B111" s="1">
+        <v>42070</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" s="6">
+        <f>SUM('Box Office'!B68:B74)</f>
+        <v>7090715</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <f t="shared" si="1"/>
+        <v>42071</v>
+      </c>
+      <c r="B112" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" s="6">
+        <f>SUM('Box Office'!B75:B81)</f>
+        <v>4703379</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <f t="shared" si="1"/>
+        <v>42078</v>
+      </c>
+      <c r="B113" s="1">
+        <v>42084</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" s="6">
+        <f>SUM('Box Office'!B82:B88)</f>
+        <v>2871166</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <f t="shared" si="1"/>
+        <v>42085</v>
+      </c>
+      <c r="B114" s="1">
+        <v>42091</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" s="6">
+        <f>SUM('Box Office'!B89:B95)</f>
+        <v>1632142</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <f t="shared" si="1"/>
+        <v>42092</v>
+      </c>
+      <c r="B115" s="1">
+        <v>42098</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115" s="6">
+        <f>SUM('Box Office'!B96:B102)</f>
+        <v>1039751</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <f t="shared" si="1"/>
+        <v>42099</v>
+      </c>
+      <c r="B116" s="1">
+        <v>42105</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" s="6">
+        <f>SUM('Box Office'!B103:B109)</f>
+        <v>847986</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <f t="shared" si="1"/>
+        <v>42106</v>
+      </c>
+      <c r="B117" s="1">
+        <v>42112</v>
+      </c>
+      <c r="C117">
+        <v>3</v>
+      </c>
+      <c r="D117" s="6">
+        <f>SUM('Box Office'!B110:B116)</f>
+        <v>574464</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <f t="shared" si="1"/>
+        <v>42113</v>
+      </c>
+      <c r="B118" s="1">
+        <v>42119</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118" s="6">
+        <f>SUM('Box Office'!B117:B123)</f>
+        <v>531415</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <f t="shared" si="1"/>
+        <v>42120</v>
+      </c>
+      <c r="B119" s="1">
+        <v>42126</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119" s="6">
+        <f>SUM('Box Office'!B124:B130)</f>
+        <v>508543</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <f t="shared" si="1"/>
+        <v>42127</v>
+      </c>
+      <c r="B120" s="1">
+        <v>42133</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" s="6">
+        <f>SUM('Box Office'!B131:B137)</f>
+        <v>526146</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <f t="shared" si="1"/>
+        <v>42134</v>
+      </c>
+      <c r="B121" s="1">
+        <v>42140</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121" s="6">
+        <f>SUM('Box Office'!B138:B144)</f>
+        <v>355872</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <f t="shared" si="1"/>
+        <v>42141</v>
+      </c>
+      <c r="B122" s="1">
+        <v>42147</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122" s="6">
+        <f>SUM('Box Office'!B145:B151)</f>
+        <v>226426</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <f t="shared" si="1"/>
+        <v>42148</v>
+      </c>
+      <c r="B123" s="1">
+        <v>42154</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123" s="6">
+        <f>SUM('Box Office'!B152:B158)</f>
+        <v>198535</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <f t="shared" si="1"/>
+        <v>42155</v>
+      </c>
+      <c r="B124" s="1">
+        <v>42161</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124" s="6">
+        <f>SUM('Box Office'!B159:B165)</f>
+        <v>64088</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <f t="shared" si="1"/>
+        <v>42162</v>
+      </c>
+      <c r="B125" s="1">
+        <v>42168</v>
+      </c>
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125" s="6">
+        <f>SUM('Box Office'!B166:B172)</f>
+        <v>24628</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <f t="shared" si="1"/>
+        <v>42169</v>
+      </c>
+      <c r="B126" s="1">
+        <v>42175</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+      <c r="D126" s="6">
+        <f>SUM('Box Office'!B173:B179)</f>
+        <v>12939</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <f t="shared" si="1"/>
+        <v>42176</v>
+      </c>
+      <c r="B127" s="1">
+        <v>42182</v>
+      </c>
+      <c r="C127">
+        <v>3</v>
+      </c>
+      <c r="D127" s="6">
+        <f>SUM('Box Office'!B180:B184)</f>
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <f t="shared" si="1"/>
+        <v>42183</v>
+      </c>
+      <c r="B128" s="1">
+        <v>42189</v>
+      </c>
+      <c r="C128">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <f t="shared" si="1"/>
+        <v>42190</v>
+      </c>
+      <c r="B129" s="1">
+        <v>42196</v>
+      </c>
+      <c r="C129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <f t="shared" si="1"/>
+        <v>42197</v>
+      </c>
+      <c r="B130" s="1">
+        <v>42203</v>
+      </c>
+      <c r="C130">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <f t="shared" si="1"/>
+        <v>42204</v>
+      </c>
+      <c r="B131" s="1">
+        <v>42210</v>
+      </c>
+      <c r="C131">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <f t="shared" ref="A132:A135" si="2">B132-6</f>
+        <v>42211</v>
+      </c>
+      <c r="B132" s="1">
+        <v>42217</v>
+      </c>
+      <c r="C132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <f t="shared" si="2"/>
+        <v>42218</v>
+      </c>
+      <c r="B133" s="1">
+        <v>42224</v>
+      </c>
+      <c r="C133">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <f t="shared" si="2"/>
+        <v>42225</v>
+      </c>
+      <c r="B134" s="1">
+        <v>42231</v>
+      </c>
+      <c r="C134">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <f t="shared" si="2"/>
+        <v>42232</v>
+      </c>
+      <c r="B135" s="1">
+        <v>42238</v>
+      </c>
+      <c r="C135">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
calculated rank and box office $ correlations
</commit_message>
<xml_diff>
--- a/1-american-sniper/american-sniper.xlsx
+++ b/1-american-sniper/american-sniper.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/1-american-sniper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6C225C6D-CECD-FB43-8F87-8D94EAD46A0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB6734CB-C088-FE43-AFD8-98E7CD1EF88F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="4160" windowWidth="22380" windowHeight="21920" activeTab="2" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
+    <workbookView xWindow="4920" yWindow="2420" windowWidth="22380" windowHeight="21920" activeTab="3" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
   </bookViews>
   <sheets>
     <sheet name="NYT Books" sheetId="1" r:id="rId1"/>
     <sheet name="Box Office" sheetId="2" r:id="rId2"/>
     <sheet name="Weekly Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Correlation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="13">
   <si>
     <t>Published Date</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>Box Office Gross</t>
+  </si>
+  <si>
+    <t>Correlation:</t>
   </si>
 </sst>
 </file>
@@ -3980,8 +3984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A462E3-9853-A64F-9EF3-EF62BAAD9838}">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101:D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5722,4 +5726,253 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D64C2F0-D6A5-2349-8ED0-0FECB09AEC30}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6">
+        <v>655550</v>
+      </c>
+      <c r="D2">
+        <f>CORREL(A2:A28,B2:B28)</f>
+        <v>-0.37611868675561838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1369410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>960761</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>65324829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>114310252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>60887363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>31787886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6">
+        <v>23971877</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6">
+        <v>18003115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6">
+        <v>11642600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6">
+        <v>7090715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>4703379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2871166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1632142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1039751</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6">
+        <v>847986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>574464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6">
+        <v>531415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6">
+        <v>508543</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6">
+        <v>526146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6">
+        <v>355872</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" s="6">
+        <v>226426</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6">
+        <v>198535</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6">
+        <v>64088</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="6">
+        <v>24628</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="6">
+        <v>12939</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4606</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished second corr calcuations
</commit_message>
<xml_diff>
--- a/1-american-sniper/american-sniper.xlsx
+++ b/1-american-sniper/american-sniper.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/1-american-sniper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsayhuth/Documents/GitHub/movies-and-their-books/1-american-sniper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB6734CB-C088-FE43-AFD8-98E7CD1EF88F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31944B7-DF66-4B42-BA00-92E007D160BB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="2420" windowWidth="22380" windowHeight="21920" activeTab="3" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="24500" windowHeight="16400" activeTab="4" xr2:uid="{AB014125-7A7F-054A-9810-5F351E6A9326}"/>
   </bookViews>
   <sheets>
     <sheet name="NYT Books" sheetId="1" r:id="rId1"/>
     <sheet name="Box Office" sheetId="2" r:id="rId2"/>
     <sheet name="Weekly Data" sheetId="3" r:id="rId3"/>
-    <sheet name="Correlation" sheetId="4" r:id="rId4"/>
+    <sheet name="Box Office $ Correlation" sheetId="4" r:id="rId4"/>
+    <sheet name="Rank + In Theaters Corr" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="15">
   <si>
     <t>Published Date</t>
   </si>
@@ -67,6 +68,12 @@
   </si>
   <si>
     <t>Correlation:</t>
+  </si>
+  <si>
+    <t>In Theaters? (1 = Y, 0 = N)</t>
+  </si>
+  <si>
+    <t>Correlation starting with first movie:</t>
   </si>
 </sst>
 </file>
@@ -118,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -126,6 +133,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +451,7 @@
   <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="B1:D1048576"/>
+      <selection sqref="A1:E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2492,7 +2500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5013F2-7369-4142-97F8-212C34FA103F}">
   <dimension ref="A1:B184"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -5732,7 +5740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D64C2F0-D6A5-2349-8ED0-0FECB09AEC30}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -5975,4 +5983,1494 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B476538E-8A7E-5D4F-A9AB-CCCF2597D833}">
+  <dimension ref="A1:F97"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <f>B2-6</f>
+        <v>41301</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41307</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>CORREL(C2:C97,D2:D97)</f>
+        <v>-0.58845902145106765</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A48" si="0">B3-6</f>
+        <v>41308</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41314</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>41315</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41321</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>41322</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41328</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>41329</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41335</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>CORREL(C63:C97,D63:D97)</f>
+        <v>-0.8344862096941168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>41336</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41342</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>41343</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41349</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>41350</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41356</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>41357</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41363</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>41364</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41370</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>41371</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41377</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>41378</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41384</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>41385</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41391</v>
+      </c>
+      <c r="C14" s="7">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>41392</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41398</v>
+      </c>
+      <c r="C15" s="7">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>41399</v>
+      </c>
+      <c r="B16" s="1">
+        <v>41405</v>
+      </c>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>41406</v>
+      </c>
+      <c r="B17" s="1">
+        <v>41412</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>41413</v>
+      </c>
+      <c r="B18" s="1">
+        <v>41419</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>41420</v>
+      </c>
+      <c r="B19" s="1">
+        <v>41426</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>41427</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41433</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>41434</v>
+      </c>
+      <c r="B21" s="1">
+        <v>41440</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>41441</v>
+      </c>
+      <c r="B22" s="1">
+        <v>41447</v>
+      </c>
+      <c r="C22" s="7">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>41448</v>
+      </c>
+      <c r="B23" s="1">
+        <v>41454</v>
+      </c>
+      <c r="C23" s="7">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>41455</v>
+      </c>
+      <c r="B24" s="1">
+        <v>41461</v>
+      </c>
+      <c r="C24" s="7">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>41462</v>
+      </c>
+      <c r="B25" s="1">
+        <v>41468</v>
+      </c>
+      <c r="C25" s="7">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>41469</v>
+      </c>
+      <c r="B26" s="1">
+        <v>41475</v>
+      </c>
+      <c r="C26" s="7">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>41476</v>
+      </c>
+      <c r="B27" s="1">
+        <v>41482</v>
+      </c>
+      <c r="C27" s="7">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>41483</v>
+      </c>
+      <c r="B28" s="1">
+        <v>41489</v>
+      </c>
+      <c r="C28" s="7">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>41490</v>
+      </c>
+      <c r="B29" s="1">
+        <v>41496</v>
+      </c>
+      <c r="C29" s="7">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>41497</v>
+      </c>
+      <c r="B30" s="1">
+        <v>41503</v>
+      </c>
+      <c r="C30" s="7">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>41560</v>
+      </c>
+      <c r="B31" s="1">
+        <v>41566</v>
+      </c>
+      <c r="C31" s="7">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>41567</v>
+      </c>
+      <c r="B32" s="1">
+        <v>41573</v>
+      </c>
+      <c r="C32" s="7">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>41588</v>
+      </c>
+      <c r="B33" s="1">
+        <v>41594</v>
+      </c>
+      <c r="C33" s="7">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>41595</v>
+      </c>
+      <c r="B34" s="1">
+        <v>41601</v>
+      </c>
+      <c r="C34" s="7">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>41602</v>
+      </c>
+      <c r="B35" s="1">
+        <v>41608</v>
+      </c>
+      <c r="C35" s="7">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>41609</v>
+      </c>
+      <c r="B36" s="1">
+        <v>41615</v>
+      </c>
+      <c r="C36" s="7">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>41616</v>
+      </c>
+      <c r="B37" s="1">
+        <v>41622</v>
+      </c>
+      <c r="C37" s="7">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>41623</v>
+      </c>
+      <c r="B38" s="1">
+        <v>41629</v>
+      </c>
+      <c r="C38" s="7">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>41630</v>
+      </c>
+      <c r="B39" s="1">
+        <v>41636</v>
+      </c>
+      <c r="C39" s="7">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>41637</v>
+      </c>
+      <c r="B40" s="1">
+        <v>41643</v>
+      </c>
+      <c r="C40" s="7">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>41644</v>
+      </c>
+      <c r="B41" s="1">
+        <v>41650</v>
+      </c>
+      <c r="C41" s="7">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>41651</v>
+      </c>
+      <c r="B42" s="1">
+        <v>41657</v>
+      </c>
+      <c r="C42" s="7">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>41658</v>
+      </c>
+      <c r="B43" s="1">
+        <v>41664</v>
+      </c>
+      <c r="C43" s="7">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>41665</v>
+      </c>
+      <c r="B44" s="1">
+        <v>41671</v>
+      </c>
+      <c r="C44" s="7">
+        <v>18</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>41672</v>
+      </c>
+      <c r="B45" s="1">
+        <v>41678</v>
+      </c>
+      <c r="C45" s="7">
+        <v>11</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>41679</v>
+      </c>
+      <c r="B46" s="1">
+        <v>41685</v>
+      </c>
+      <c r="C46" s="7">
+        <v>11</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>41686</v>
+      </c>
+      <c r="B47" s="1">
+        <v>41692</v>
+      </c>
+      <c r="C47" s="7">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>41693</v>
+      </c>
+      <c r="B48" s="1">
+        <v>41699</v>
+      </c>
+      <c r="C48" s="7">
+        <v>19</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" ref="A49:A92" si="1">B49-6</f>
+        <v>41847</v>
+      </c>
+      <c r="B49" s="1">
+        <v>41853</v>
+      </c>
+      <c r="C49" s="7">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="1"/>
+        <v>41868</v>
+      </c>
+      <c r="B50" s="1">
+        <v>41874</v>
+      </c>
+      <c r="C50" s="7">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="1"/>
+        <v>41910</v>
+      </c>
+      <c r="B51" s="1">
+        <v>41916</v>
+      </c>
+      <c r="C51" s="7">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="1"/>
+        <v>41917</v>
+      </c>
+      <c r="B52" s="1">
+        <v>41923</v>
+      </c>
+      <c r="C52" s="7">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="1"/>
+        <v>41924</v>
+      </c>
+      <c r="B53" s="1">
+        <v>41930</v>
+      </c>
+      <c r="C53" s="7">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="1"/>
+        <v>41931</v>
+      </c>
+      <c r="B54" s="1">
+        <v>41937</v>
+      </c>
+      <c r="C54" s="7">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="1"/>
+        <v>41938</v>
+      </c>
+      <c r="B55" s="1">
+        <v>41944</v>
+      </c>
+      <c r="C55" s="7">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="1"/>
+        <v>41945</v>
+      </c>
+      <c r="B56" s="1">
+        <v>41951</v>
+      </c>
+      <c r="C56" s="7">
+        <v>9</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="1"/>
+        <v>41952</v>
+      </c>
+      <c r="B57" s="1">
+        <v>41958</v>
+      </c>
+      <c r="C57" s="7">
+        <v>5</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="1"/>
+        <v>41959</v>
+      </c>
+      <c r="B58" s="1">
+        <v>41965</v>
+      </c>
+      <c r="C58" s="7">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="1"/>
+        <v>41966</v>
+      </c>
+      <c r="B59" s="1">
+        <v>41972</v>
+      </c>
+      <c r="C59" s="7">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="1"/>
+        <v>41973</v>
+      </c>
+      <c r="B60" s="1">
+        <v>41979</v>
+      </c>
+      <c r="C60" s="7">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="1"/>
+        <v>41980</v>
+      </c>
+      <c r="B61" s="1">
+        <v>41986</v>
+      </c>
+      <c r="C61" s="7">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="1"/>
+        <v>41987</v>
+      </c>
+      <c r="B62" s="1">
+        <v>41993</v>
+      </c>
+      <c r="C62" s="7">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="1"/>
+        <v>41994</v>
+      </c>
+      <c r="B63" s="1">
+        <v>42000</v>
+      </c>
+      <c r="C63" s="7">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="1"/>
+        <v>42001</v>
+      </c>
+      <c r="B64" s="1">
+        <v>42007</v>
+      </c>
+      <c r="C64" s="7">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="1"/>
+        <v>42008</v>
+      </c>
+      <c r="B65" s="1">
+        <v>42014</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="1"/>
+        <v>42015</v>
+      </c>
+      <c r="B66" s="1">
+        <v>42021</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="1"/>
+        <v>42022</v>
+      </c>
+      <c r="B67" s="1">
+        <v>42028</v>
+      </c>
+      <c r="C67" s="7">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" si="1"/>
+        <v>42029</v>
+      </c>
+      <c r="B68" s="1">
+        <v>42035</v>
+      </c>
+      <c r="C68" s="7">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>42036</v>
+      </c>
+      <c r="B69" s="1">
+        <v>42042</v>
+      </c>
+      <c r="C69" s="7">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>42043</v>
+      </c>
+      <c r="B70" s="1">
+        <v>42049</v>
+      </c>
+      <c r="C70" s="7">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>42050</v>
+      </c>
+      <c r="B71" s="1">
+        <v>42056</v>
+      </c>
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>42057</v>
+      </c>
+      <c r="B72" s="1">
+        <v>42063</v>
+      </c>
+      <c r="C72" s="7">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <f t="shared" si="1"/>
+        <v>42064</v>
+      </c>
+      <c r="B73" s="1">
+        <v>42070</v>
+      </c>
+      <c r="C73" s="7">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>42071</v>
+      </c>
+      <c r="B74" s="1">
+        <v>42077</v>
+      </c>
+      <c r="C74" s="7">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>42078</v>
+      </c>
+      <c r="B75" s="1">
+        <v>42084</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>42085</v>
+      </c>
+      <c r="B76" s="1">
+        <v>42091</v>
+      </c>
+      <c r="C76" s="7">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>42092</v>
+      </c>
+      <c r="B77" s="1">
+        <v>42098</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>42099</v>
+      </c>
+      <c r="B78" s="1">
+        <v>42105</v>
+      </c>
+      <c r="C78" s="7">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>42106</v>
+      </c>
+      <c r="B79" s="1">
+        <v>42112</v>
+      </c>
+      <c r="C79" s="7">
+        <v>3</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" si="1"/>
+        <v>42113</v>
+      </c>
+      <c r="B80" s="1">
+        <v>42119</v>
+      </c>
+      <c r="C80" s="7">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="1"/>
+        <v>42120</v>
+      </c>
+      <c r="B81" s="1">
+        <v>42126</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="1"/>
+        <v>42127</v>
+      </c>
+      <c r="B82" s="1">
+        <v>42133</v>
+      </c>
+      <c r="C82" s="7">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="1"/>
+        <v>42134</v>
+      </c>
+      <c r="B83" s="1">
+        <v>42140</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="1"/>
+        <v>42141</v>
+      </c>
+      <c r="B84" s="1">
+        <v>42147</v>
+      </c>
+      <c r="C84" s="7">
+        <v>2</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="1"/>
+        <v>42148</v>
+      </c>
+      <c r="B85" s="1">
+        <v>42154</v>
+      </c>
+      <c r="C85" s="7">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="1"/>
+        <v>42155</v>
+      </c>
+      <c r="B86" s="1">
+        <v>42161</v>
+      </c>
+      <c r="C86" s="7">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="1"/>
+        <v>42162</v>
+      </c>
+      <c r="B87" s="1">
+        <v>42168</v>
+      </c>
+      <c r="C87" s="7">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="1"/>
+        <v>42169</v>
+      </c>
+      <c r="B88" s="1">
+        <v>42175</v>
+      </c>
+      <c r="C88" s="7">
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="1"/>
+        <v>42176</v>
+      </c>
+      <c r="B89" s="1">
+        <v>42182</v>
+      </c>
+      <c r="C89" s="7">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <f t="shared" si="1"/>
+        <v>42183</v>
+      </c>
+      <c r="B90" s="1">
+        <v>42189</v>
+      </c>
+      <c r="C90" s="7">
+        <v>6</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <f t="shared" si="1"/>
+        <v>42190</v>
+      </c>
+      <c r="B91" s="1">
+        <v>42196</v>
+      </c>
+      <c r="C91" s="7">
+        <v>9</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <f t="shared" si="1"/>
+        <v>42197</v>
+      </c>
+      <c r="B92" s="1">
+        <v>42203</v>
+      </c>
+      <c r="C92" s="7">
+        <v>5</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <f t="shared" ref="A93:A97" si="2">B93-6</f>
+        <v>42204</v>
+      </c>
+      <c r="B93" s="1">
+        <v>42210</v>
+      </c>
+      <c r="C93" s="7">
+        <v>6</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <f t="shared" si="2"/>
+        <v>42211</v>
+      </c>
+      <c r="B94" s="1">
+        <v>42217</v>
+      </c>
+      <c r="C94" s="7">
+        <v>5</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <f t="shared" si="2"/>
+        <v>42218</v>
+      </c>
+      <c r="B95" s="1">
+        <v>42224</v>
+      </c>
+      <c r="C95" s="7">
+        <v>14</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <f t="shared" si="2"/>
+        <v>42225</v>
+      </c>
+      <c r="B96" s="1">
+        <v>42231</v>
+      </c>
+      <c r="C96" s="7">
+        <v>14</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <f t="shared" si="2"/>
+        <v>42232</v>
+      </c>
+      <c r="B97" s="1">
+        <v>42238</v>
+      </c>
+      <c r="C97" s="7">
+        <v>12</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>